<commit_message>
Added notes to template, improved error data
git-tfs-id: [http://mlwweb05:8080/tfs/defaultcollection]$/Footlocker.Logistics/Allocation/Main;C35779
</commit_message>
<xml_diff>
--- a/Allocation/Footlocker.Logistics.Allocation/Content/Templates/BulkRangeTemplate.xlsx
+++ b/Allocation/Footlocker.Logistics.Allocation/Content/Templates/BulkRangeTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://footlocker-my.sharepoint.com/personal/u695130_footlocker_com/Documents/Documents/Working Copy Code/Allocation/Development/XLS Upgrade/Allocation/Footlocker.Logistics.Allocation/Content/Templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://footlocker-my.sharepoint.com/personal/u695130_footlocker_com/Documents/Documents/Working Copy Code/Allocation/Main/Allocation/Footlocker.Logistics.Allocation/Content/Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BF59DCA5-933D-4408-8381-CF095449401C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{BF59DCA5-933D-4408-8381-CF095449401C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{04CA01AF-971E-4F6E-B264-FE41B04CF275}"/>
   <bookViews>
-    <workbookView xWindow="6585" yWindow="1140" windowWidth="28125" windowHeight="16650"/>
+    <workbookView xWindow="4485" yWindow="2490" windowWidth="26805" windowHeight="16425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,93 +18,17 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>Christopher Dick</author>
     <author>Frank Schmitt</author>
-    <author>Christopher Dick</author>
   </authors>
   <commentList>
-    <comment ref="E1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>##-##-#####-##</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Enter "ALL" if you want all sizes of the sku.  Min/Max/etc will be applied to all sizes.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>This is the start date of the delivery group.  If a delivery group already exists for this date, it will be added.  If not, it will be created.  The actual start date will be this date plus lead time days.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Optional</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="M1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>optional.  If populated, existing record will be updated with end date.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="N1" authorId="1" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{1E9F4D7E-BE05-482E-95DE-993E0E0CC557}">
       <text>
         <r>
           <rPr>
@@ -114,7 +38,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Date to start sending to Order Planning. Must be in format MM/DD/YYYY</t>
+          <t>Mandatory field. Format: ##</t>
         </r>
         <r>
           <rPr>
@@ -128,7 +52,72 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="1" shapeId="0">
+    <comment ref="E1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>##-##-#####-##</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Enter "ALL" if you want all sizes of the sku.  Min/Max/etc will be applied to all sizes.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>This is the start date of the delivery group.  If a delivery group already exists for this date, it will be added.  If not, it will be created.  The actual start date will be this date plus lead time days. This should be in a MM/DD/YYYY format.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Optional</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>optional.  If populated, existing record will be updated with end date. This should be in a MM/DD/YYYY format.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -138,7 +127,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Date to stop sending to Order Planning. Must be in format MM/DD/YYYY</t>
+          <t>Date to start sending to Order Planning. Must be in format MM/DD/YYYY</t>
         </r>
         <r>
           <rPr>
@@ -152,7 +141,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="1" shapeId="0">
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -162,7 +151,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Freeform text to describe Order Planning range. Should be less than 50 characters.</t>
+          <t>Date to stop sending to Order Planning. Must be in format MM/DD/YYYY</t>
         </r>
         <r>
           <rPr>
@@ -176,6 +165,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Freeform text to describe Order Planning range. Should be less than 50 characters.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -234,7 +247,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -292,9 +305,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -310,6 +325,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -598,7 +617,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -607,6 +626,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="4" width="9.140625" style="3"/>
+    <col min="5" max="5" width="19.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="3"/>
     <col min="7" max="7" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
@@ -618,22 +640,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -678,7 +700,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -694,7 +716,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>